<commit_message>
minor changes to ipam und cli
- removed router in "router und switch adressen"
- added "do copy running-config startup-config" to router and swtich in cli
</commit_message>
<xml_diff>
--- a/IPAM-LF09.xlsx
+++ b/IPAM-LF09.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxim\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5F689B-9F39-4BB0-A8E1-0CA59F912057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9551BC-E71E-4BD5-A2CE-5E7CBDD9250E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{0C367987-59E3-4F3C-8BEA-0D34FF592100}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0C367987-59E3-4F3C-8BEA-0D34FF592100}"/>
   </bookViews>
   <sheets>
     <sheet name="Adressplan &amp; VLAN-Adressen" sheetId="2" r:id="rId1"/>
-    <sheet name="RT+SW  &amp; Client+Server Adressen" sheetId="3" r:id="rId2"/>
+    <sheet name="SW  &amp; Client+Server Adressen" sheetId="3" r:id="rId2"/>
     <sheet name="Transportnetz-Adressen" sheetId="5" r:id="rId3"/>
     <sheet name="Statische Routen" sheetId="6" state="hidden" r:id="rId4"/>
     <sheet name="Portbelegung" sheetId="7" r:id="rId5"/>
@@ -468,9 +468,6 @@
     <t>Adressplan</t>
   </si>
   <si>
-    <t>Router- und Switch-Adressen</t>
-  </si>
-  <si>
     <t>PC</t>
   </si>
   <si>
@@ -712,6 +709,9 @@
   </si>
   <si>
     <t>2001:db8:D60::/64</t>
+  </si>
+  <si>
+    <t>Switch-Adressen</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1068,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1516,7 +1516,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1538,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -1583,10 +1583,10 @@
       <c r="Q2" s="11"/>
     </row>
     <row r="3" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="9"/>
+      <c r="A3" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="10"/>
       <c r="C3" s="16" t="s">
         <v>3</v>
       </c>
@@ -1601,30 +1601,30 @@
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L3" s="14"/>
       <c r="M3" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="10"/>
+      <c r="A4" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="9"/>
       <c r="C4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="G4" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="G4" s="9" t="s">
         <v>124</v>
       </c>
       <c r="H4" s="6"/>
@@ -1633,30 +1633,30 @@
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="9"/>
+      <c r="A5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="10"/>
       <c r="C5" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="G5" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>125</v>
       </c>
       <c r="H5" s="8"/>
@@ -1665,30 +1665,30 @@
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
     </row>
     <row r="6" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B6" s="10"/>
+      <c r="A6" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="9"/>
       <c r="C6" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="G6" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="G6" s="9" t="s">
         <v>125</v>
       </c>
       <c r="H6" s="6"/>
@@ -1697,30 +1697,30 @@
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B7" s="9"/>
+      <c r="A7" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="10"/>
       <c r="C7" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="G7" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="G7" s="10" t="s">
         <v>126</v>
       </c>
       <c r="H7" s="8"/>
@@ -1729,30 +1729,30 @@
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
     </row>
     <row r="8" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B8" s="10"/>
+      <c r="A8" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="G8" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="G8" s="9" t="s">
         <v>127</v>
       </c>
       <c r="H8" s="6"/>
@@ -1761,175 +1761,175 @@
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
     </row>
     <row r="9" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="B9" s="9"/>
+      <c r="A9" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="10"/>
       <c r="C9" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+        <v>200</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="B10" s="10"/>
+      <c r="A10" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="9"/>
       <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" s="9"/>
+      <c r="A11" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="10"/>
       <c r="C11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="B12" s="10"/>
+      <c r="A12" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="9"/>
       <c r="C12" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" s="9"/>
+      <c r="A13" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="10"/>
       <c r="C13" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="B14" s="10"/>
+      <c r="A14" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="9"/>
       <c r="C14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B15" s="9"/>
+      <c r="A15" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="10"/>
       <c r="C15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B16" s="10"/>
+      <c r="A16" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="9"/>
       <c r="C16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="9"/>
+      <c r="A17" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="10"/>
       <c r="C17" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B18" s="10"/>
+      <c r="A18" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="9"/>
       <c r="C18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="B19" s="9"/>
+      <c r="A19" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="10"/>
       <c r="C19" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B20" s="10"/>
+      <c r="A20" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="9"/>
       <c r="C20" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="82">
@@ -2026,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C19E1F8-EBDF-475C-ABFA-B0924175ABEA}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2039,7 +2039,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>142</v>
+        <v>223</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2088,156 +2088,156 @@
         <v>17</v>
       </c>
       <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="8"/>
-      <c r="I3" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="J3" s="9"/>
+      <c r="I3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="K3" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="L3" s="9"/>
+        <v>154</v>
+      </c>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="5" t="s">
         <v>28</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="J4" s="10"/>
+      <c r="I4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J4" s="9"/>
       <c r="K4" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="L4" s="10"/>
+        <v>155</v>
+      </c>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="8"/>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H5" s="8"/>
-      <c r="I5" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="J5" s="9"/>
+      <c r="I5" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="J5" s="10"/>
       <c r="K5" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="L5" s="9"/>
+        <v>156</v>
+      </c>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="J6" s="10"/>
+      <c r="I6" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J6" s="9"/>
       <c r="K6" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="L6" s="10"/>
+        <v>157</v>
+      </c>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H7" s="8"/>
-      <c r="I7" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="J7" s="9"/>
+      <c r="I7" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="J7" s="10"/>
       <c r="K7" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="L7" s="9"/>
+        <v>158</v>
+      </c>
+      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="J8" s="10"/>
+      <c r="I8" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J8" s="9"/>
       <c r="K8" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="L8" s="10"/>
+        <v>159</v>
+      </c>
+      <c r="L8" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="16" t="s">
@@ -2291,25 +2291,25 @@
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="5" t="s">
@@ -2317,25 +2317,25 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J13" s="6"/>
-      <c r="K13" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="L13" s="10"/>
+      <c r="K13" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="7" t="s">
@@ -2343,25 +2343,25 @@
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J14" s="8"/>
-      <c r="K14" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="L14" s="9"/>
+      <c r="K14" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="10"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="5" t="s">
@@ -2369,69 +2369,69 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="L15" s="10"/>
+      <c r="K15" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J16" s="8"/>
-      <c r="K16" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="L16" s="9"/>
+      <c r="K16" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="10"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J17" s="6"/>
-      <c r="K17" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="L17" s="10"/>
+      <c r="K17" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="L17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="86">
@@ -2447,12 +2447,12 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="G17:H17"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="I13:J13"/>
@@ -2464,6 +2464,8 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="I12:J12"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -2494,18 +2496,15 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="I12:J12"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="A1:L1"/>
@@ -2521,6 +2520,7 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2530,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C264FEC-7202-414F-91B4-973A059B06E2}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10:M10"/>
     </sheetView>
   </sheetViews>
@@ -2560,11 +2560,11 @@
         <v>30</v>
       </c>
       <c r="J1" s="26"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
     </row>
     <row r="2" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -2575,448 +2575,448 @@
         <v>19</v>
       </c>
       <c r="D2" s="14"/>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H2" s="14"/>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="10"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="8"/>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H4" s="8"/>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="9"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J5" s="10"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H6" s="8"/>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="9"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H8" s="8"/>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="9"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H10" s="8"/>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
     </row>
     <row r="11" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H12" s="8"/>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="J13" s="10"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H14" s="8"/>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="10"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="10"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="9"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="10"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="J17" s="10"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="9"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="J18" s="9"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="10"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="10"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H19" s="6"/>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="10"/>
+      <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="9"/>
+      <c r="F20" s="10"/>
       <c r="G20" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H20" s="8"/>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J20" s="9"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="10"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="10"/>
+      <c r="F21" s="9"/>
       <c r="G21" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="J21" s="10"/>
+      <c r="J21" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="111">
@@ -3458,78 +3458,78 @@
       <c r="Q2" s="37"/>
     </row>
     <row r="3" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="33" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="34"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="35" t="s">
         <v>121</v>
       </c>
       <c r="H3" s="36"/>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="K3" s="9"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="33" t="s">
         <v>19</v>
       </c>
       <c r="M3" s="34"/>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="9"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="35" t="s">
         <v>128</v>
       </c>
       <c r="Q3" s="36"/>
     </row>
     <row r="4" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="30"/>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="31" t="s">
         <v>120</v>
       </c>
       <c r="H4" s="32"/>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="10"/>
+      <c r="K4" s="9"/>
       <c r="L4" s="29" t="s">
         <v>35</v>
       </c>
       <c r="M4" s="30"/>
-      <c r="N4" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="O4" s="10"/>
+      <c r="N4" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="O4" s="9"/>
       <c r="P4" s="31" t="s">
         <v>129</v>
       </c>
       <c r="Q4" s="32"/>
     </row>
     <row r="5" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="33" t="s">
         <v>22</v>
       </c>
@@ -3542,16 +3542,16 @@
         <v>122</v>
       </c>
       <c r="H5" s="42"/>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K5" s="9"/>
+      <c r="K5" s="10"/>
       <c r="L5" s="33" t="s">
         <v>36</v>
       </c>
       <c r="M5" s="34"/>
       <c r="N5" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O5" s="34"/>
       <c r="P5" s="41" t="s">
@@ -3560,28 +3560,28 @@
       <c r="Q5" s="42"/>
     </row>
     <row r="6" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="29" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="30"/>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="31" t="s">
         <v>123</v>
       </c>
       <c r="H6" s="32"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
       <c r="L6" s="29"/>
       <c r="M6" s="30"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
       <c r="P6" s="31"/>
       <c r="Q6" s="32"/>
     </row>
@@ -3643,130 +3643,130 @@
       <c r="Q8" s="37"/>
     </row>
     <row r="9" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="33" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="34"/>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="35" t="s">
         <v>128</v>
       </c>
       <c r="H9" s="36"/>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="K9" s="9"/>
+      <c r="K9" s="10"/>
       <c r="L9" s="33" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="34"/>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="O9" s="9"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="35" t="s">
         <v>120</v>
       </c>
       <c r="Q9" s="36"/>
     </row>
     <row r="10" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="29" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="30"/>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="31" t="s">
         <v>131</v>
       </c>
       <c r="H10" s="32"/>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="K10" s="10"/>
+      <c r="K10" s="9"/>
       <c r="L10" s="29" t="s">
         <v>37</v>
       </c>
       <c r="M10" s="30"/>
-      <c r="N10" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="O10" s="10"/>
+      <c r="N10" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="O10" s="9"/>
       <c r="P10" s="31" t="s">
         <v>133</v>
       </c>
       <c r="Q10" s="32"/>
     </row>
     <row r="11" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="33" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="34"/>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="41" t="s">
         <v>123</v>
       </c>
       <c r="H11" s="42"/>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K11" s="9"/>
+      <c r="K11" s="10"/>
       <c r="L11" s="33" t="s">
         <v>38</v>
       </c>
       <c r="M11" s="34"/>
-      <c r="N11" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="O11" s="9"/>
+      <c r="N11" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="O11" s="10"/>
       <c r="P11" s="41" t="s">
         <v>134</v>
       </c>
       <c r="Q11" s="42"/>
     </row>
     <row r="12" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="30"/>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="31" t="s">
         <v>122</v>
       </c>
       <c r="H12" s="32"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="29"/>
       <c r="M12" s="30"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
       <c r="P12" s="31"/>
       <c r="Q12" s="32"/>
     </row>
@@ -3828,122 +3828,122 @@
       <c r="Q14" s="37"/>
     </row>
     <row r="15" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="9"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="33" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="34"/>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="9"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="35" t="s">
         <v>128</v>
       </c>
       <c r="H15" s="36"/>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="10"/>
       <c r="L15" s="33" t="s">
         <v>21</v>
       </c>
       <c r="M15" s="34"/>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="O15" s="9"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="35" t="s">
         <v>123</v>
       </c>
       <c r="Q15" s="36"/>
     </row>
     <row r="16" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="10"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="30"/>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="31" t="s">
         <v>120</v>
       </c>
       <c r="H16" s="32"/>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="K16" s="10"/>
+      <c r="K16" s="9"/>
       <c r="L16" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="M16" s="30"/>
+      <c r="N16" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="O16" s="9"/>
+      <c r="P16" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="M16" s="30"/>
-      <c r="N16" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="O16" s="10"/>
-      <c r="P16" s="31" t="s">
-        <v>206</v>
-      </c>
       <c r="Q16" s="32"/>
     </row>
     <row r="17" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="33" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="34"/>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="41" t="s">
         <v>132</v>
       </c>
       <c r="H17" s="42"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
       <c r="L17" s="33"/>
       <c r="M17" s="34"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
       <c r="P17" s="41"/>
       <c r="Q17" s="42"/>
     </row>
     <row r="18" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="10"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="30"/>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="31" t="s">
         <v>122</v>
       </c>
       <c r="H18" s="32"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
       <c r="L18" s="29"/>
       <c r="M18" s="30"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="32"/>
     </row>
@@ -4005,122 +4005,122 @@
       <c r="Q20" s="37"/>
     </row>
     <row r="21" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="9"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="33" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="34"/>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F21" s="9"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="35" t="s">
         <v>128</v>
       </c>
       <c r="H21" s="36"/>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="K21" s="9"/>
+      <c r="K21" s="10"/>
       <c r="L21" s="33" t="s">
         <v>22</v>
       </c>
       <c r="M21" s="34"/>
-      <c r="N21" s="9" t="s">
+      <c r="N21" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="O21" s="9"/>
+      <c r="O21" s="10"/>
       <c r="P21" s="35" t="s">
         <v>122</v>
       </c>
       <c r="Q21" s="36"/>
     </row>
     <row r="22" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="10"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="30"/>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="10"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="31" t="s">
         <v>120</v>
       </c>
       <c r="H22" s="32"/>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="K22" s="10"/>
+      <c r="K22" s="9"/>
       <c r="L22" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M22" s="30"/>
-      <c r="N22" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="O22" s="10"/>
+      <c r="N22" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="O22" s="9"/>
       <c r="P22" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q22" s="32"/>
     </row>
     <row r="23" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="33" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="34"/>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="41" t="s">
         <v>123</v>
       </c>
       <c r="H23" s="42"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
       <c r="L23" s="33"/>
       <c r="M23" s="34"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
       <c r="P23" s="41"/>
       <c r="Q23" s="42"/>
     </row>
     <row r="24" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="10"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="30"/>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="31" t="s">
         <v>135</v>
       </c>
       <c r="H24" s="32"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
       <c r="L24" s="29"/>
       <c r="M24" s="30"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
       <c r="P24" s="31"/>
       <c r="Q24" s="32"/>
     </row>
@@ -4182,41 +4182,41 @@
       <c r="Q26" s="37"/>
     </row>
     <row r="27" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="9"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="33" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="34"/>
-      <c r="E27" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F27" s="9"/>
+      <c r="E27" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F27" s="10"/>
       <c r="G27" s="35" t="s">
         <v>121</v>
       </c>
       <c r="H27" s="36"/>
-      <c r="J27" s="9" t="s">
+      <c r="J27" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="K27" s="9"/>
+      <c r="K27" s="10"/>
       <c r="L27" s="33" t="s">
         <v>23</v>
       </c>
       <c r="M27" s="34"/>
-      <c r="N27" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="O27" s="9"/>
+      <c r="N27" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="O27" s="10"/>
       <c r="P27" s="35" t="s">
         <v>121</v>
       </c>
       <c r="Q27" s="36"/>
     </row>
     <row r="28" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="30"/>
       <c r="C28" s="29"/>
       <c r="D28" s="30"/>
@@ -4224,7 +4224,7 @@
       <c r="F28" s="30"/>
       <c r="G28" s="31"/>
       <c r="H28" s="32"/>
-      <c r="J28" s="10"/>
+      <c r="J28" s="9"/>
       <c r="K28" s="30"/>
       <c r="L28" s="29"/>
       <c r="M28" s="30"/>
@@ -4291,41 +4291,41 @@
       <c r="Q30" s="37"/>
     </row>
     <row r="31" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="33" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="34"/>
-      <c r="E31" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="F31" s="9"/>
+      <c r="E31" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F31" s="10"/>
       <c r="G31" s="35" t="s">
         <v>131</v>
       </c>
       <c r="H31" s="36"/>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="K31" s="9"/>
+      <c r="K31" s="10"/>
       <c r="L31" s="33" t="s">
         <v>24</v>
       </c>
       <c r="M31" s="34"/>
-      <c r="N31" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="O31" s="9"/>
+      <c r="N31" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="O31" s="10"/>
       <c r="P31" s="35" t="s">
         <v>131</v>
       </c>
       <c r="Q31" s="36"/>
     </row>
     <row r="32" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="30"/>
       <c r="C32" s="29"/>
       <c r="D32" s="30"/>
@@ -4333,7 +4333,7 @@
       <c r="F32" s="30"/>
       <c r="G32" s="31"/>
       <c r="H32" s="32"/>
-      <c r="J32" s="10"/>
+      <c r="J32" s="9"/>
       <c r="K32" s="30"/>
       <c r="L32" s="29"/>
       <c r="M32" s="30"/>
@@ -4344,7 +4344,7 @@
     </row>
     <row r="33" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
@@ -4355,7 +4355,7 @@
       <c r="H33" s="26"/>
       <c r="I33" s="3"/>
       <c r="J33" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K33" s="26"/>
       <c r="L33" s="26"/>
@@ -4400,41 +4400,41 @@
       <c r="Q34" s="37"/>
     </row>
     <row r="35" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B35" s="9"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="33" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="34"/>
-      <c r="E35" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="F35" s="9"/>
+      <c r="E35" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="10"/>
       <c r="G35" s="35" t="s">
         <v>132</v>
       </c>
       <c r="H35" s="36"/>
-      <c r="J35" s="9" t="s">
+      <c r="J35" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="K35" s="9"/>
+      <c r="K35" s="10"/>
       <c r="L35" s="33" t="s">
         <v>26</v>
       </c>
       <c r="M35" s="34"/>
-      <c r="N35" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="O35" s="9"/>
+      <c r="N35" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="O35" s="10"/>
       <c r="P35" s="35" t="s">
         <v>135</v>
       </c>
       <c r="Q35" s="36"/>
     </row>
     <row r="36" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="30"/>
       <c r="C36" s="29"/>
       <c r="D36" s="30"/>
@@ -4442,7 +4442,7 @@
       <c r="F36" s="30"/>
       <c r="G36" s="31"/>
       <c r="H36" s="32"/>
-      <c r="J36" s="10"/>
+      <c r="J36" s="9"/>
       <c r="K36" s="30"/>
       <c r="L36" s="29"/>
       <c r="M36" s="30"/>

</xml_diff>